<commit_message>
Added the Actor and Use Case description. Added the Use case summaries
</commit_message>
<xml_diff>
--- a/Feature Matrix.xlsx
+++ b/Feature Matrix.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
   <si>
     <t>Feature #</t>
   </si>
@@ -169,13 +169,45 @@
   </si>
   <si>
     <t>View/PerformTreatmentPlans</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Legend:</t>
+  </si>
+  <si>
+    <t>Indicates system feature not belonging to use case</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">X - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Indicates a relationship between feature and use case</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,13 +242,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -270,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -278,14 +331,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,16 +626,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E4:AK23"/>
+  <dimension ref="B4:AK23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection activeCell="F1" sqref="F1"/>
+      <selection pane="topRight" activeCell="AK21" sqref="AK21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="5.5234375" customWidth="1"/>
-    <col min="3" max="3" width="4.5234375" customWidth="1"/>
+    <col min="2" max="2" width="44.83984375" customWidth="1"/>
+    <col min="3" max="3" width="19.89453125" customWidth="1"/>
     <col min="4" max="4" width="6.89453125" customWidth="1"/>
     <col min="5" max="5" width="3.7890625" customWidth="1"/>
     <col min="6" max="6" width="16.47265625" customWidth="1"/>
@@ -612,116 +674,118 @@
     <col min="37" max="37" width="11.5234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="6:37" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="G4" s="6" t="s">
+    <row r="4" spans="2:37" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="G4" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="6:37" ht="30.9" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="F5" s="6" t="s">
+    <row r="5" spans="2:37" ht="30.9" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="F5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="P5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="Q5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="R5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="S5" s="5" t="s">
+      <c r="S5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="T5" s="5" t="s">
+      <c r="T5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="U5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="V5" s="5" t="s">
+      <c r="V5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="W5" s="5" t="s">
+      <c r="W5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="X5" s="5" t="s">
+      <c r="X5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Y5" s="5" t="s">
+      <c r="Y5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Z5" s="5" t="s">
+      <c r="Z5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AA5" s="5" t="s">
+      <c r="AA5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AB5" s="5" t="s">
+      <c r="AB5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AC5" s="5" t="s">
+      <c r="AC5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AD5" s="5" t="s">
+      <c r="AD5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AE5" s="5" t="s">
+      <c r="AE5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AF5" s="5" t="s">
+      <c r="AF5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AG5" s="5" t="s">
+      <c r="AG5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AH5" s="5" t="s">
+      <c r="AH5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AI5" s="5" t="s">
+      <c r="AI5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AJ5" s="5" t="s">
+      <c r="AJ5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AK5" s="5" t="s">
+      <c r="AK5" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="6:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="G6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="3"/>
+      <c r="H6" s="6"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="L6" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -740,19 +804,19 @@
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
-      <c r="AE6" s="2"/>
-      <c r="AF6" s="2"/>
-      <c r="AG6" s="2"/>
-      <c r="AH6" s="2"/>
+      <c r="AE6" s="8"/>
+      <c r="AF6" s="8"/>
+      <c r="AG6" s="8"/>
+      <c r="AH6" s="8"/>
       <c r="AI6" s="2"/>
       <c r="AJ6" s="2"/>
       <c r="AK6" s="2"/>
     </row>
-    <row r="7" spans="6:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="7" spans="2:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="G7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="4"/>
+      <c r="H7" s="7"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -775,19 +839,26 @@
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
-      <c r="AE7" s="2"/>
-      <c r="AF7" s="2"/>
-      <c r="AG7" s="2"/>
-      <c r="AH7" s="2"/>
-      <c r="AI7" s="2"/>
-      <c r="AJ7" s="2"/>
+      <c r="AE7" s="8"/>
+      <c r="AF7" s="8"/>
+      <c r="AG7" s="8"/>
+      <c r="AH7" s="8"/>
+      <c r="AI7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ7" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="AK7" s="2"/>
     </row>
-    <row r="8" spans="6:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="8" spans="2:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
       <c r="G8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="4"/>
+      <c r="H8" s="7"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -796,7 +867,9 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
+      <c r="Q8" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
@@ -810,19 +883,22 @@
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
-      <c r="AE8" s="2"/>
-      <c r="AF8" s="2"/>
-      <c r="AG8" s="2"/>
-      <c r="AH8" s="2"/>
+      <c r="AE8" s="8"/>
+      <c r="AF8" s="8"/>
+      <c r="AG8" s="8"/>
+      <c r="AH8" s="8"/>
       <c r="AI8" s="2"/>
       <c r="AJ8" s="2"/>
       <c r="AK8" s="2"/>
     </row>
-    <row r="9" spans="6:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="9" spans="2:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B9" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="G9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="4"/>
+      <c r="H9" s="7"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -830,12 +906,18 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
+      <c r="P9" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
+      <c r="R9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="S9" s="5"/>
       <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
+      <c r="U9" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
@@ -845,19 +927,22 @@
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
       <c r="AD9" s="2"/>
-      <c r="AE9" s="2"/>
-      <c r="AF9" s="2"/>
-      <c r="AG9" s="2"/>
-      <c r="AH9" s="2"/>
+      <c r="AE9" s="8"/>
+      <c r="AF9" s="8"/>
+      <c r="AG9" s="8"/>
+      <c r="AH9" s="8"/>
       <c r="AI9" s="2"/>
       <c r="AJ9" s="2"/>
       <c r="AK9" s="2"/>
     </row>
-    <row r="10" spans="6:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="2:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
       <c r="G10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="4"/>
+      <c r="H10" s="7"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -869,9 +954,11 @@
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
+      <c r="T10" s="5"/>
       <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
+      <c r="V10" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
@@ -880,19 +967,19 @@
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
-      <c r="AE10" s="2"/>
-      <c r="AF10" s="2"/>
-      <c r="AG10" s="2"/>
-      <c r="AH10" s="2"/>
+      <c r="AE10" s="8"/>
+      <c r="AF10" s="8"/>
+      <c r="AG10" s="8"/>
+      <c r="AH10" s="8"/>
       <c r="AI10" s="2"/>
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2"/>
     </row>
-    <row r="11" spans="6:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="11" spans="2:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="G11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="4"/>
+      <c r="H11" s="7"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -903,8 +990,12 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
+      <c r="S11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="T11" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
@@ -915,19 +1006,19 @@
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
-      <c r="AE11" s="2"/>
-      <c r="AF11" s="2"/>
-      <c r="AG11" s="2"/>
-      <c r="AH11" s="2"/>
+      <c r="AE11" s="8"/>
+      <c r="AF11" s="8"/>
+      <c r="AG11" s="8"/>
+      <c r="AH11" s="8"/>
       <c r="AI11" s="2"/>
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
     </row>
-    <row r="12" spans="6:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="2:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="G12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="4"/>
+      <c r="H12" s="7"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -942,7 +1033,9 @@
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
+      <c r="W12" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
@@ -950,19 +1043,19 @@
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
       <c r="AD12" s="2"/>
-      <c r="AE12" s="2"/>
-      <c r="AF12" s="2"/>
-      <c r="AG12" s="2"/>
-      <c r="AH12" s="2"/>
+      <c r="AE12" s="8"/>
+      <c r="AF12" s="8"/>
+      <c r="AG12" s="8"/>
+      <c r="AH12" s="8"/>
       <c r="AI12" s="2"/>
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
     </row>
-    <row r="13" spans="6:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="13" spans="2:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="G13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="4"/>
+      <c r="H13" s="7"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -978,26 +1071,32 @@
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
-      <c r="X13" s="2"/>
+      <c r="X13" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
-      <c r="AB13" s="2"/>
+      <c r="AB13" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="AC13" s="2"/>
-      <c r="AD13" s="2"/>
-      <c r="AE13" s="2"/>
-      <c r="AF13" s="2"/>
-      <c r="AG13" s="2"/>
-      <c r="AH13" s="2"/>
+      <c r="AD13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE13" s="8"/>
+      <c r="AF13" s="8"/>
+      <c r="AG13" s="8"/>
+      <c r="AH13" s="8"/>
       <c r="AI13" s="2"/>
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
     </row>
-    <row r="14" spans="6:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="2:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="G14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="4"/>
+      <c r="H14" s="7"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -1018,21 +1117,23 @@
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
-      <c r="AC14" s="2"/>
+      <c r="AC14" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="AD14" s="2"/>
-      <c r="AE14" s="2"/>
-      <c r="AF14" s="2"/>
-      <c r="AG14" s="2"/>
-      <c r="AH14" s="2"/>
+      <c r="AE14" s="8"/>
+      <c r="AF14" s="8"/>
+      <c r="AG14" s="8"/>
+      <c r="AH14" s="8"/>
       <c r="AI14" s="2"/>
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
     </row>
-    <row r="15" spans="6:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="15" spans="2:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="G15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H15" s="4"/>
+      <c r="H15" s="7"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -1055,19 +1156,19 @@
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
       <c r="AD15" s="2"/>
-      <c r="AE15" s="2"/>
-      <c r="AF15" s="2"/>
-      <c r="AG15" s="2"/>
-      <c r="AH15" s="2"/>
+      <c r="AE15" s="8"/>
+      <c r="AF15" s="8"/>
+      <c r="AG15" s="8"/>
+      <c r="AH15" s="8"/>
       <c r="AI15" s="2"/>
       <c r="AJ15" s="2"/>
       <c r="AK15" s="2"/>
     </row>
-    <row r="16" spans="6:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="2:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="G16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H16" s="4"/>
+      <c r="H16" s="7"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -1090,10 +1191,10 @@
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
       <c r="AD16" s="2"/>
-      <c r="AE16" s="2"/>
-      <c r="AF16" s="2"/>
-      <c r="AG16" s="2"/>
-      <c r="AH16" s="2"/>
+      <c r="AE16" s="8"/>
+      <c r="AF16" s="8"/>
+      <c r="AG16" s="8"/>
+      <c r="AH16" s="8"/>
       <c r="AI16" s="2"/>
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
@@ -1102,13 +1203,15 @@
       <c r="G17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H17" s="2"/>
+      <c r="H17" s="8"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
+      <c r="N17" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
@@ -1125,10 +1228,10 @@
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
       <c r="AD17" s="2"/>
-      <c r="AE17" s="2"/>
-      <c r="AF17" s="2"/>
-      <c r="AG17" s="2"/>
-      <c r="AH17" s="2"/>
+      <c r="AE17" s="8"/>
+      <c r="AF17" s="8"/>
+      <c r="AG17" s="8"/>
+      <c r="AH17" s="8"/>
       <c r="AI17" s="2"/>
       <c r="AJ17" s="2"/>
       <c r="AK17" s="2"/>
@@ -1137,14 +1240,18 @@
       <c r="G18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H18" s="2"/>
+      <c r="H18" s="8"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
+      <c r="M18" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
+      <c r="O18" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
@@ -1160,10 +1267,10 @@
       <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
       <c r="AD18" s="2"/>
-      <c r="AE18" s="2"/>
-      <c r="AF18" s="2"/>
-      <c r="AG18" s="2"/>
-      <c r="AH18" s="2"/>
+      <c r="AE18" s="8"/>
+      <c r="AF18" s="8"/>
+      <c r="AG18" s="8"/>
+      <c r="AH18" s="8"/>
       <c r="AI18" s="2"/>
       <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
@@ -1172,10 +1279,14 @@
       <c r="G19" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -1195,10 +1306,10 @@
       <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
       <c r="AD19" s="2"/>
-      <c r="AE19" s="2"/>
-      <c r="AF19" s="2"/>
-      <c r="AG19" s="2"/>
-      <c r="AH19" s="2"/>
+      <c r="AE19" s="8"/>
+      <c r="AF19" s="8"/>
+      <c r="AG19" s="8"/>
+      <c r="AH19" s="8"/>
       <c r="AI19" s="2"/>
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
@@ -1207,10 +1318,10 @@
       <c r="G20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H20" s="2"/>
+      <c r="H20" s="8"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
+      <c r="K20" s="5"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -1221,19 +1332,25 @@
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
+      <c r="V20" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
-      <c r="Z20" s="2"/>
-      <c r="AA20" s="2"/>
+      <c r="Z20" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA20" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="AB20" s="2"/>
       <c r="AC20" s="2"/>
       <c r="AD20" s="2"/>
-      <c r="AE20" s="2"/>
-      <c r="AF20" s="2"/>
-      <c r="AG20" s="2"/>
-      <c r="AH20" s="2"/>
+      <c r="AE20" s="8"/>
+      <c r="AF20" s="8"/>
+      <c r="AG20" s="8"/>
+      <c r="AH20" s="8"/>
       <c r="AI20" s="2"/>
       <c r="AJ20" s="2"/>
       <c r="AK20" s="2"/>
@@ -1242,7 +1359,7 @@
       <c r="G21" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H21" s="2"/>
+      <c r="H21" s="8"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -1265,21 +1382,27 @@
       <c r="AB21" s="2"/>
       <c r="AC21" s="2"/>
       <c r="AD21" s="2"/>
-      <c r="AE21" s="2"/>
-      <c r="AF21" s="2"/>
-      <c r="AG21" s="2"/>
-      <c r="AH21" s="2"/>
+      <c r="AE21" s="8"/>
+      <c r="AF21" s="8"/>
+      <c r="AG21" s="8"/>
+      <c r="AH21" s="8"/>
       <c r="AI21" s="2"/>
       <c r="AJ21" s="2"/>
-      <c r="AK21" s="2"/>
+      <c r="AK21" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="22" spans="7:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="G22" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
@@ -1300,10 +1423,10 @@
       <c r="AB22" s="2"/>
       <c r="AC22" s="2"/>
       <c r="AD22" s="2"/>
-      <c r="AE22" s="2"/>
-      <c r="AF22" s="2"/>
-      <c r="AG22" s="2"/>
-      <c r="AH22" s="2"/>
+      <c r="AE22" s="8"/>
+      <c r="AF22" s="8"/>
+      <c r="AG22" s="8"/>
+      <c r="AH22" s="8"/>
       <c r="AI22" s="2"/>
       <c r="AJ22" s="2"/>
       <c r="AK22" s="2"/>
@@ -1312,7 +1435,7 @@
       <c r="G23" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H23" s="2"/>
+      <c r="H23" s="8"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -1329,16 +1452,18 @@
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
       <c r="X23" s="2"/>
-      <c r="Y23" s="2"/>
+      <c r="Y23" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
       <c r="AD23" s="2"/>
-      <c r="AE23" s="2"/>
-      <c r="AF23" s="2"/>
-      <c r="AG23" s="2"/>
-      <c r="AH23" s="2"/>
+      <c r="AE23" s="8"/>
+      <c r="AF23" s="8"/>
+      <c r="AG23" s="8"/>
+      <c r="AH23" s="8"/>
       <c r="AI23" s="2"/>
       <c r="AJ23" s="2"/>
       <c r="AK23" s="2"/>

</xml_diff>

<commit_message>
Added Robert Northmore's part and Craig Cook's part to the SRS document
</commit_message>
<xml_diff>
--- a/Feature Matrix.xlsx
+++ b/Feature Matrix.xlsx
@@ -628,10 +628,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:AK23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F11" workbookViewId="0">
       <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="topRight" activeCell="AK21" sqref="AK21"/>
+      <selection pane="topRight" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>